<commit_message>
Add analysis for single school
</commit_message>
<xml_diff>
--- a/data_analysis/questionnaire_answers.xlsx
+++ b/data_analysis/questionnaire_answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fasteno/code/Evaluation_paper/data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1B3E36-8623-C444-AB1B-861F80692667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D3882E-76E1-724E-8A3E-83FE422856EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{22BF4857-3568-2045-A6C7-AFC5B8E0F0B7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{22BF4857-3568-2045-A6C7-AFC5B8E0F0B7}"/>
   </bookViews>
   <sheets>
     <sheet name="SALESIANOS" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -554,7 +554,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2292,7 +2291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF58F5F-0C7F-604D-9958-1D16F7A69CC7}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:M1"/>
     </sheetView>
   </sheetViews>
@@ -3275,10 +3274,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF24B11B-41D8-D841-B254-34F03B905242}">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3291,7 +3290,7 @@
     <col min="17" max="23" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>33</v>
       </c>
@@ -3356,7 +3355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -3420,11 +3419,8 @@
       <c r="U2" s="20">
         <v>5</v>
       </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-    </row>
-    <row r="3" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -3488,11 +3484,8 @@
       <c r="U3" s="20">
         <v>4</v>
       </c>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33"/>
-    </row>
-    <row r="4" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -3556,11 +3549,8 @@
       <c r="U4" s="20">
         <v>4</v>
       </c>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-    </row>
-    <row r="5" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -3624,11 +3614,8 @@
       <c r="U5" s="20">
         <v>3</v>
       </c>
-      <c r="X5" s="33"/>
-      <c r="Y5" s="33"/>
-      <c r="Z5" s="33"/>
-    </row>
-    <row r="6" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -3692,11 +3679,8 @@
       <c r="U6" s="20">
         <v>3</v>
       </c>
-      <c r="X6" s="33"/>
-      <c r="Y6" s="33"/>
-      <c r="Z6" s="33"/>
-    </row>
-    <row r="7" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -3760,11 +3744,8 @@
       <c r="U7" s="20">
         <v>4</v>
       </c>
-      <c r="X7" s="33"/>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="33"/>
-    </row>
-    <row r="8" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -3828,11 +3809,8 @@
       <c r="U8" s="20">
         <v>4</v>
       </c>
-      <c r="X8" s="33"/>
-      <c r="Y8" s="33"/>
-      <c r="Z8" s="33"/>
-    </row>
-    <row r="9" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -3896,11 +3874,8 @@
       <c r="U9" s="20">
         <v>4</v>
       </c>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="33"/>
-      <c r="Z9" s="33"/>
-    </row>
-    <row r="10" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -3964,11 +3939,8 @@
       <c r="U10" s="20">
         <v>3</v>
       </c>
-      <c r="X10" s="33"/>
-      <c r="Y10" s="33"/>
-      <c r="Z10" s="33"/>
-    </row>
-    <row r="11" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -4032,11 +4004,8 @@
       <c r="U11" s="20">
         <v>4</v>
       </c>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="33"/>
-      <c r="Z11" s="33"/>
-    </row>
-    <row r="12" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -4100,11 +4069,8 @@
       <c r="U12" s="20">
         <v>3</v>
       </c>
-      <c r="X12" s="33"/>
-      <c r="Y12" s="33"/>
-      <c r="Z12" s="33"/>
-    </row>
-    <row r="13" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -4168,11 +4134,8 @@
       <c r="U13" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="X13" s="33"/>
-      <c r="Y13" s="33"/>
-      <c r="Z13" s="33"/>
-    </row>
-    <row r="14" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -4236,11 +4199,8 @@
       <c r="U14" s="20">
         <v>3</v>
       </c>
-      <c r="X14" s="33"/>
-      <c r="Y14" s="33"/>
-      <c r="Z14" s="33"/>
-    </row>
-    <row r="15" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -4304,11 +4264,8 @@
       <c r="U15" s="20">
         <v>4</v>
       </c>
-      <c r="X15" s="33"/>
-      <c r="Y15" s="33"/>
-      <c r="Z15" s="33"/>
-    </row>
-    <row r="16" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -4372,11 +4329,8 @@
       <c r="U16" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="X16" s="33"/>
-      <c r="Y16" s="33"/>
-      <c r="Z16" s="33"/>
-    </row>
-    <row r="17" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -4440,11 +4394,8 @@
       <c r="U17" s="20">
         <v>2</v>
       </c>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
-    </row>
-    <row r="18" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -4508,11 +4459,8 @@
       <c r="U18" s="20">
         <v>4</v>
       </c>
-      <c r="X18" s="33"/>
-      <c r="Y18" s="33"/>
-      <c r="Z18" s="33"/>
-    </row>
-    <row r="19" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -4576,11 +4524,8 @@
       <c r="U19" s="20">
         <v>5</v>
       </c>
-      <c r="X19" s="33"/>
-      <c r="Y19" s="33"/>
-      <c r="Z19" s="33"/>
-    </row>
-    <row r="20" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -4644,11 +4589,8 @@
       <c r="U20" s="20">
         <v>4</v>
       </c>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-    </row>
-    <row r="21" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -4712,67 +4654,64 @@
       <c r="U21" s="20">
         <v>4</v>
       </c>
-      <c r="X21" s="33"/>
-      <c r="Y21" s="33"/>
-      <c r="Z21" s="33"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C30" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="33" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="33" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improving data analysis all data
</commit_message>
<xml_diff>
--- a/data_analysis/questionnaire_answers.xlsx
+++ b/data_analysis/questionnaire_answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fasteno/code/Evaluation_paper/data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D3882E-76E1-724E-8A3E-83FE422856EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91D11F0-8E80-5941-861B-E88108BDDACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{22BF4857-3568-2045-A6C7-AFC5B8E0F0B7}"/>
+    <workbookView xWindow="34440" yWindow="640" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{22BF4857-3568-2045-A6C7-AFC5B8E0F0B7}"/>
   </bookViews>
   <sheets>
     <sheet name="SALESIANOS" sheetId="1" r:id="rId1"/>
@@ -2292,7 +2292,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:M1"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>